<commit_message>
Update Palorsennan Train Lines.xlsx
</commit_message>
<xml_diff>
--- a/Palorsenna/Palorsennan Train Lines.xlsx
+++ b/Palorsenna/Palorsennan Train Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\OneDrive\Documents\Worldbuilding\Englishia Politica\6DES-Pol\Palorsenna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011D5443-2C61-47D7-855B-585C7B894D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46007C60-227F-419D-B345-508C27318ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Line Name</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Purpose</t>
-  </si>
-  <si>
-    <t>High Speed Passenger Transportation, Freight</t>
   </si>
   <si>
     <t>Ownership</t>
@@ -173,19 +170,46 @@
     <t>Donland-Solder</t>
   </si>
   <si>
-    <t>Snubavik- Bofoker</t>
-  </si>
-  <si>
     <t>The Riverlands Line</t>
   </si>
   <si>
-    <t>2 Medium Speed</t>
-  </si>
-  <si>
     <t>Low Speed Passenger Transportation, Freight</t>
   </si>
   <si>
-    <t>Medium Speed Passenger Transportation</t>
+    <t>2 High Speed</t>
+  </si>
+  <si>
+    <t>High Speed Passenger Transportation</t>
+  </si>
+  <si>
+    <t>Very High Speed Passenger Transportation, Freight</t>
+  </si>
+  <si>
+    <t>Snubavik-Bofoker</t>
+  </si>
+  <si>
+    <t>Snubavik-Gravden-Lokernes-Kjersnes-Barbakvik-Laufargar-Bofoker</t>
+  </si>
+  <si>
+    <t>Bofoker-Grimsjahver</t>
+  </si>
+  <si>
+    <t>Raunahild-Rivervo-Raupige</t>
+  </si>
+  <si>
+    <t>The Capital Line</t>
+  </si>
+  <si>
+    <t>Raunahild-Raupige</t>
+  </si>
+  <si>
+    <t>Raupige-Raupige</t>
+  </si>
+  <si>
+    <t>Raupige-Snubavik-Karldalla-Raupige</t>
+  </si>
+  <si>
+    <t>The Lake Line</t>
   </si>
 </sst>
 </file>
@@ -529,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -542,7 +566,7 @@
     <col min="3" max="3" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -552,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -567,21 +591,24 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -589,143 +616,180 @@
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>